<commit_message>
Exported Excel and PDF mapping spreadsheets
</commit_message>
<xml_diff>
--- a/Mapping_Spreadsheets/00_Crash_Driver_Report_Fresh.xlsx
+++ b/Mapping_Spreadsheets/00_Crash_Driver_Report_Fresh.xlsx
@@ -668,7 +668,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -698,7 +697,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -724,7 +722,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -750,7 +747,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -776,7 +772,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -802,7 +797,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -828,7 +822,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -854,7 +847,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -880,7 +872,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -906,7 +897,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -957,7 +947,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -983,7 +972,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1009,7 +997,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1035,7 +1022,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1061,7 +1047,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1087,7 +1072,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1113,7 +1097,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1139,7 +1122,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1165,7 +1147,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1191,7 +1172,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1239,7 +1219,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1269,7 +1248,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1295,7 +1273,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1321,7 +1298,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1347,7 +1323,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1373,7 +1348,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1399,7 +1373,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1425,7 +1398,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1451,7 +1423,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
@@ -1477,7 +1448,6 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:tabLst/>
           <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>

</xml_diff>